<commit_message>
Mise a jour explication maquette + Backlog
</commit_message>
<xml_diff>
--- a/docs/planning/TF_PlanificationProjet.xlsx
+++ b/docs/planning/TF_PlanificationProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\PHP\ProjectTPI\docs\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6818E3B3-5D19-4E28-8238-6F5876FB01F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE2095E-0F41-41AB-BF31-F846C4BC19F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="1635" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -247,12 +247,6 @@
     <t>Système de notation des itinéraires</t>
   </si>
   <si>
-    <t>Modification du status de l'itinéraire</t>
-  </si>
-  <si>
-    <t>Modification du status de l'utilisateur</t>
-  </si>
-  <si>
     <t>Supression d'un itinéraire</t>
   </si>
   <si>
@@ -271,9 +265,6 @@
     <t>Affichage informations itinéraire</t>
   </si>
   <si>
-    <t>Affichage informations utilisateur</t>
-  </si>
-  <si>
     <t>Création du MCD</t>
   </si>
   <si>
@@ -284,6 +275,15 @@
   </si>
   <si>
     <t>Ajout/Modification des informations personnelles d'un utilisateur</t>
+  </si>
+  <si>
+    <t>Modification du statut de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Affichage profil utilisateur</t>
+  </si>
+  <si>
+    <t>Modification du statut de l'itinéraire</t>
   </si>
 </sst>
 </file>
@@ -4726,8 +4726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5325,7 +5325,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B25" s="7">
         <v>8.3333333333333329E-2</v>
@@ -5471,7 +5471,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B31" s="7">
         <v>8.3333333333333329E-2</v>
@@ -5496,7 +5496,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B32" s="7">
         <v>4.1666666666666664E-2</v>
@@ -5542,7 +5542,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B34" s="7">
         <v>4.1666666666666664E-2</v>
@@ -5591,7 +5591,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B36" s="7">
         <v>8.3333333333333329E-2</v>
@@ -5737,7 +5737,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B42" s="7">
         <v>8.3333333333333329E-2</v>
@@ -5764,7 +5764,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B43" s="7">
         <v>4.1666666666666664E-2</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B45" s="7">
         <v>4.1666666666666664E-2</v>
@@ -5856,7 +5856,7 @@
     </row>
     <row r="47" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B47" s="15">
         <v>4.1666666666666664E-2</v>
@@ -5878,7 +5878,7 @@
     </row>
     <row r="48" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B48" s="15">
         <v>4.1666666666666664E-2</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="51" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B51" s="15">
         <v>4.1666666666666664E-2</v>
@@ -5994,7 +5994,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B53" s="7">
         <v>4.1666666666666664E-2</v>
@@ -6017,7 +6017,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B54" s="7">
         <v>4.1666666666666664E-2</v>

</xml_diff>